<commit_message>
insert user in database
</commit_message>
<xml_diff>
--- a/database/dictionary.xlsx
+++ b/database/dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\adnan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\adnan\source\slrrmods\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37089AF9-36F0-4874-8600-F71E6A6F4B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC30824-3410-432E-A539-8E8CF0412A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{06EC9EF5-EB63-4559-9811-ECF5A250585D}"/>
   </bookViews>
@@ -45,7 +45,6 @@
     <sheet name="ForumReply" sheetId="32" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="196">
   <si>
     <t>User</t>
   </si>
@@ -125,39 +124,15 @@
     <t>text</t>
   </si>
   <si>
-    <t>first_login</t>
-  </si>
-  <si>
-    <t>last_login</t>
-  </si>
-  <si>
     <t>profile_picture</t>
   </si>
   <si>
-    <t>confirmed</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
-    <t>confirmed_at</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>confirmation_sent_at</t>
-  </si>
-  <si>
-    <t>if the user has confirmed his email</t>
-  </si>
-  <si>
-    <t>when the email was confirmated</t>
-  </si>
-  <si>
-    <t>when the email confirmation was sent</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -651,6 +626,33 @@
   </si>
   <si>
     <t>moderator</t>
+  </si>
+  <si>
+    <t>when then user was created</t>
+  </si>
+  <si>
+    <t>last_sign_in_at</t>
+  </si>
+  <si>
+    <t>the last time that this user has changed it's informations</t>
+  </si>
+  <si>
+    <t>email_confirmation_sent_at</t>
+  </si>
+  <si>
+    <t>email_confirmation_token</t>
+  </si>
+  <si>
+    <t>email_confirmed_at</t>
+  </si>
+  <si>
+    <t>password_recovery_sent_at</t>
+  </si>
+  <si>
+    <t>password_recovery_token</t>
+  </si>
+  <si>
+    <t>password_recovered_at</t>
   </si>
 </sst>
 </file>
@@ -710,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -727,6 +729,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2246,8 +2249,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1687C86F-431A-4D7C-B6AB-C42452DC4EB7}" name="Tabela1" displayName="Tabela1" ref="A2:I18" totalsRowShown="0" headerRowDxfId="299" dataDxfId="298">
-  <autoFilter ref="A2:I18" xr:uid="{1687C86F-431A-4D7C-B6AB-C42452DC4EB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1687C86F-431A-4D7C-B6AB-C42452DC4EB7}" name="Tabela1" displayName="Tabela1" ref="A2:I23" totalsRowShown="0" headerRowDxfId="299" dataDxfId="298">
+  <autoFilter ref="A2:I23" xr:uid="{1687C86F-431A-4D7C-B6AB-C42452DC4EB7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3CE6E30F-E1BE-4EA7-8388-1D081F667119}" name="Field" dataDxfId="297"/>
     <tableColumn id="2" xr3:uid="{905D48EE-DAA6-471F-A925-8EF51EE64A59}" name="Type" dataDxfId="296"/>
@@ -3030,15 +3036,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D64F4C7-B4C2-44A5-9769-B07F1FB738D3}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.125" style="2" bestFit="1" customWidth="1"/>
@@ -3088,15 +3094,15 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -3108,10 +3114,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
@@ -3119,22 +3125,22 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>32</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -3145,33 +3151,36 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -3180,13 +3189,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="2">
-        <v>2048</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -3197,7 +3206,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -3209,36 +3218,33 @@
         <v>10</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
       </c>
       <c r="E8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -3255,7 +3261,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -3274,20 +3280,23 @@
       </c>
       <c r="H9" s="4">
         <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -3304,19 +3313,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>181</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6000</v>
       </c>
       <c r="E11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -3326,43 +3335,37 @@
       </c>
       <c r="H11" s="4">
         <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>32</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
@@ -3374,7 +3377,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
@@ -3386,12 +3389,12 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>188</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -3414,16 +3417,13 @@
       <c r="H14" s="4">
         <v>0</v>
       </c>
-      <c r="I14" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -3442,26 +3442,29 @@
       </c>
       <c r="H15" s="4">
         <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>256</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -3470,21 +3473,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>100</v>
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
@@ -3496,18 +3499,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2">
-        <v>6000</v>
+        <v>1024</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -3521,6 +3524,137 @@
       <c r="H18" s="4">
         <v>0</v>
       </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1024</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1024</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3557,7 +3691,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3594,12 +3728,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -3623,12 +3757,12 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -3652,12 +3786,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -3683,10 +3817,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -3707,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3744,7 +3878,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3781,12 +3915,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -3812,7 +3946,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -3836,12 +3970,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -3867,7 +4001,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -3893,7 +4027,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -3919,7 +4053,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -3943,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3980,7 +4114,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -4017,12 +4151,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -4046,12 +4180,12 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -4075,12 +4209,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -4106,10 +4240,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -4164,7 +4298,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -4201,12 +4335,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -4232,7 +4366,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -4256,12 +4390,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -4287,7 +4421,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -4313,7 +4447,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -4339,7 +4473,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
@@ -4365,7 +4499,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -4389,15 +4523,15 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -4420,10 +4554,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -4446,7 +4580,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
@@ -4472,7 +4606,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -4496,15 +4630,15 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -4559,7 +4693,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -4596,12 +4730,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -4627,7 +4761,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -4685,7 +4819,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -4722,12 +4856,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -4751,12 +4885,12 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -4780,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -4817,7 +4951,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -4854,12 +4988,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -4885,7 +5019,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -4909,12 +5043,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -4940,10 +5074,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -4966,7 +5100,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -4990,15 +5124,15 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -5053,7 +5187,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5090,12 +5224,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -5121,7 +5255,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -5179,7 +5313,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5216,12 +5350,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -5247,7 +5381,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
@@ -5273,7 +5407,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -5297,15 +5431,15 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -5328,7 +5462,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
@@ -5354,7 +5488,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -5378,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -5415,7 +5549,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5452,15 +5586,15 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -5515,7 +5649,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5552,12 +5686,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -5583,7 +5717,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -5609,7 +5743,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -5635,7 +5769,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -5653,15 +5787,15 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -5684,10 +5818,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -5710,10 +5844,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -5736,10 +5870,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -5762,10 +5896,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -5820,7 +5954,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5857,12 +5991,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -5886,7 +6020,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -5923,7 +6057,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5960,12 +6094,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -5989,15 +6123,15 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -6020,7 +6154,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -6046,7 +6180,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -6070,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -6107,7 +6241,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6144,12 +6278,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -6175,7 +6309,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -6201,7 +6335,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -6227,10 +6361,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -6285,7 +6419,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6322,12 +6456,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -6353,7 +6487,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -6379,10 +6513,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -6405,7 +6539,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -6429,12 +6563,12 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -6458,7 +6592,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -6495,7 +6629,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6532,12 +6666,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -6563,7 +6697,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -6589,7 +6723,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -6615,7 +6749,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -6641,7 +6775,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -6665,12 +6799,12 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
@@ -6694,15 +6828,15 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -6725,10 +6859,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -6751,16 +6885,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -6777,10 +6911,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -6835,7 +6969,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6872,12 +7006,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -6903,7 +7037,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -6927,15 +7061,15 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -6990,7 +7124,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7027,12 +7161,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -7056,12 +7190,12 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -7085,15 +7219,15 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -7116,7 +7250,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -7142,7 +7276,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -7166,7 +7300,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -7203,7 +7337,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7240,12 +7374,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -7303,7 +7437,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7340,12 +7474,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -7371,7 +7505,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -7395,15 +7529,15 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -7426,7 +7560,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -7452,7 +7586,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -7476,15 +7610,15 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -7539,7 +7673,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7576,12 +7710,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -7607,7 +7741,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -7633,10 +7767,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -7691,7 +7825,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7728,12 +7862,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -7757,12 +7891,12 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -7786,12 +7920,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -7817,7 +7951,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -7841,12 +7975,12 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -7872,7 +8006,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -7896,15 +8030,15 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -7959,7 +8093,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7996,12 +8130,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -8025,7 +8159,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -8062,7 +8196,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -8099,12 +8233,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -8130,7 +8264,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -8156,7 +8290,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -8180,7 +8314,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -8217,7 +8351,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -8254,12 +8388,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -8285,7 +8419,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -8309,12 +8443,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -8340,7 +8474,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -8366,7 +8500,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -8392,10 +8526,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -8451,7 +8585,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -8488,12 +8622,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -8519,7 +8653,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -8543,12 +8677,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -8574,7 +8708,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -8598,12 +8732,12 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -8629,7 +8763,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
@@ -8655,7 +8789,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -8679,12 +8813,12 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
@@ -8743,7 +8877,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -8780,12 +8914,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -8811,7 +8945,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -8835,12 +8969,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -8864,12 +8998,12 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -8895,7 +9029,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
@@ -8921,7 +9055,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
@@ -8947,7 +9081,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -8971,7 +9105,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -9009,7 +9143,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -9046,12 +9180,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -9077,7 +9211,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -9136,7 +9270,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -9173,12 +9307,12 @@
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -9204,7 +9338,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -9230,7 +9364,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -9256,7 +9390,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -9280,21 +9414,21 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>

</xml_diff>